<commit_message>
Small change to the fetching data function
</commit_message>
<xml_diff>
--- a/Solina/Production/Results_Production_xgb.xlsx
+++ b/Solina/Production/Results_Production_xgb.xlsx
@@ -25,9 +25,6 @@
     <t>Prediction</t>
   </si>
   <si>
-    <t>2024-03-21</t>
-  </si>
-  <si>
     <t>2024-03-22</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>2024-03-29</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="2">
-        <v>0.5384859442710876</v>
+        <v>0.531111478805542</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -420,7 +420,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>0.4742761850357056</v>
+        <v>0.5527240633964539</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -431,7 +431,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2">
-        <v>0.4638195633888245</v>
+        <v>0.4280891418457031</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -442,7 +442,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2">
-        <v>0.2903875410556793</v>
+        <v>0.2591042816638947</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -453,7 +453,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="2">
-        <v>0.1386508196592331</v>
+        <v>0.1504656076431274</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -464,7 +464,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>0.05714630708098412</v>
+        <v>0.06011993438005447</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -475,7 +475,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="2">
-        <v>0.00961021427065134</v>
+        <v>0.009618937037885189</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -486,7 +486,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2">
-        <v>0.00157602597028017</v>
+        <v>0.001596485148184001</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -497,7 +497,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2">
-        <v>0.001550646615214646</v>
+        <v>0.001596485148184001</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -508,7 +508,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="2">
-        <v>0.001550646615214646</v>
+        <v>0.00157602597028017</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -519,7 +519,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="2">
-        <v>0.001473839627578855</v>
+        <v>0.001498213154263794</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -530,7 +530,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="2">
-        <v>0.001473839627578855</v>
+        <v>0.001498213154263794</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -541,7 +541,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="2">
-        <v>0.001501603168435395</v>
+        <v>0.001498213154263794</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>0.001818391028791666</v>
+        <v>0.001758344937115908</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="2">
-        <v>0.001818391028791666</v>
+        <v>0.001758344937115908</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -574,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="2">
-        <v>0.001818391028791666</v>
+        <v>0.001758344937115908</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -585,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>0.001709290081635118</v>
+        <v>0.001820396166294813</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -596,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2">
-        <v>0.001709290081635118</v>
+        <v>0.001820396166294813</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -607,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="2">
-        <v>0.008319715969264507</v>
+        <v>0.009711515158414841</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -618,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="2">
-        <v>0.04097757488489151</v>
+        <v>0.03872333094477654</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -629,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="2">
-        <v>0.1034688875079155</v>
+        <v>0.1275391280651093</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -640,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="2">
-        <v>0.1758942604064941</v>
+        <v>0.3109587728977203</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -651,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="C24" s="2">
-        <v>0.2961312234401703</v>
+        <v>0.3965180814266205</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
       <c r="C25" s="2">
-        <v>0.4123645722866058</v>
+        <v>0.5021463632583618</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="2">
-        <v>0.4652583301067352</v>
+        <v>0.5473080277442932</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -684,7 +684,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="2">
-        <v>0.3813600242137909</v>
+        <v>0.5518757104873657</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -695,7 +695,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="2">
-        <v>0.2965265810489655</v>
+        <v>0.4413212239742279</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -706,7 +706,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="2">
-        <v>0.2483923435211182</v>
+        <v>0.337122917175293</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -717,7 +717,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="2">
-        <v>0.1257508546113968</v>
+        <v>0.2171129137277603</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -728,7 +728,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="2">
-        <v>0.0535883717238903</v>
+        <v>0.08976252377033234</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -739,7 +739,7 @@
         <v>17</v>
       </c>
       <c r="C32" s="2">
-        <v>0.009652157314121723</v>
+        <v>0.01414182223379612</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -750,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="C33" s="2">
-        <v>0.001595305162481964</v>
+        <v>0.001606028061360121</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -761,7 +761,7 @@
         <v>19</v>
       </c>
       <c r="C34" s="2">
-        <v>0.001574845984578133</v>
+        <v>0.001501958351582289</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -772,7 +772,7 @@
         <v>20</v>
       </c>
       <c r="C35" s="2">
-        <v>0.001547082210890949</v>
+        <v>0.001501958351582289</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -783,7 +783,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="2">
-        <v>0.001497388002462685</v>
+        <v>0.001419755863025784</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -794,7 +794,7 @@
         <v>22</v>
       </c>
       <c r="C37" s="2">
-        <v>0.001497388002462685</v>
+        <v>0.001419755863025784</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -805,7 +805,7 @@
         <v>23</v>
       </c>
       <c r="C38" s="2">
-        <v>0.001503608305938542</v>
+        <v>0.001419755863025784</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.001735456753522158</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.001735456753522158</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="2">
-        <v>0.001820396166294813</v>
+        <v>0.001829984015785158</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -849,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="2">
-        <v>0.001820396166294813</v>
+        <v>0.001801040023565292</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -860,7 +860,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2">
-        <v>0.001816024538129568</v>
+        <v>0.001747380709275603</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -871,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="2">
-        <v>0.0118530485779047</v>
+        <v>0.008163020014762878</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -882,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="2">
-        <v>0.07375132292509079</v>
+        <v>0.03103868290781975</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -893,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="2">
-        <v>0.1660571098327637</v>
+        <v>0.08109454065561295</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -904,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="2">
-        <v>0.3102226555347443</v>
+        <v>0.1491440683603287</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -915,7 +915,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="2">
-        <v>0.4281874299049377</v>
+        <v>0.2794862687587738</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -926,7 +926,7 @@
         <v>10</v>
       </c>
       <c r="C49" s="2">
-        <v>0.5153080821037292</v>
+        <v>0.3724546730518341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -937,7 +937,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="2">
-        <v>0.5310064554214478</v>
+        <v>0.3133758306503296</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
       <c r="C51" s="2">
-        <v>0.5521663427352905</v>
+        <v>0.2397262752056122</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -959,7 +959,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="2">
-        <v>0.4511509239673615</v>
+        <v>0.1865478008985519</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -970,7 +970,7 @@
         <v>14</v>
       </c>
       <c r="C53" s="2">
-        <v>0.372549295425415</v>
+        <v>0.1299076229333878</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -981,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="C54" s="2">
-        <v>0.2198164612054825</v>
+        <v>0.06683869659900665</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -992,7 +992,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="2">
-        <v>0.1095724925398827</v>
+        <v>0.03296571597456932</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1003,7 +1003,7 @@
         <v>17</v>
       </c>
       <c r="C56" s="2">
-        <v>0.0147703941911459</v>
+        <v>0.01277642976492643</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1014,7 +1014,7 @@
         <v>18</v>
       </c>
       <c r="C57" s="2">
-        <v>0.001606028061360121</v>
+        <v>0.001582328230142593</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1025,7 +1025,7 @@
         <v>19</v>
       </c>
       <c r="C58" s="2">
-        <v>0.001501958351582289</v>
+        <v>0.001582328230142593</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1036,7 +1036,7 @@
         <v>20</v>
       </c>
       <c r="C59" s="2">
-        <v>0.001501958351582289</v>
+        <v>0.001582328230142593</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1047,7 +1047,7 @@
         <v>21</v>
       </c>
       <c r="C60" s="2">
-        <v>0.001515107695013285</v>
+        <v>0.001500125625170767</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1058,7 +1058,7 @@
         <v>22</v>
       </c>
       <c r="C61" s="2">
-        <v>0.001515107695013285</v>
+        <v>0.001479919767007232</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1069,7 +1069,7 @@
         <v>23</v>
       </c>
       <c r="C62" s="2">
-        <v>0.001494648749940097</v>
+        <v>0.001479919767007232</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="2">
-        <v>0.001749385381117463</v>
+        <v>0.001756184617988765</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="2">
-        <v>0.001749385381117463</v>
+        <v>0.001756184617988765</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1102,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="2">
-        <v>0.001749385381117463</v>
+        <v>0.001745106419548392</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="2">
-        <v>0.001748560694977641</v>
+        <v>0.001709290081635118</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1124,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="C67" s="2">
-        <v>0.001748560694977641</v>
+        <v>0.001681526424363256</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1135,7 +1135,7 @@
         <v>5</v>
       </c>
       <c r="C68" s="2">
-        <v>0.007956649176776409</v>
+        <v>0.009383793920278549</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1146,7 +1146,7 @@
         <v>6</v>
       </c>
       <c r="C69" s="2">
-        <v>0.0352025218307972</v>
+        <v>0.04251806437969208</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1157,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="2">
-        <v>0.08275077491998672</v>
+        <v>0.1151808798313141</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1168,7 +1168,7 @@
         <v>8</v>
       </c>
       <c r="C71" s="2">
-        <v>0.1636277437210083</v>
+        <v>0.2080928087234497</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1179,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="C72" s="2">
-        <v>0.2769133150577545</v>
+        <v>0.2761012315750122</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1190,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="C73" s="2">
-        <v>0.3294275104999542</v>
+        <v>0.4675039947032928</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1201,7 +1201,7 @@
         <v>11</v>
       </c>
       <c r="C74" s="2">
-        <v>0.4022562801837921</v>
+        <v>0.4026133120059967</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1212,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="C75" s="2">
-        <v>0.3425118625164032</v>
+        <v>0.4187763035297394</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1223,7 +1223,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="2">
-        <v>0.3099372684955597</v>
+        <v>0.3243970274925232</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1234,7 +1234,7 @@
         <v>14</v>
       </c>
       <c r="C77" s="2">
-        <v>0.2171440422534943</v>
+        <v>0.2554626762866974</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1245,7 +1245,7 @@
         <v>15</v>
       </c>
       <c r="C78" s="2">
-        <v>0.1400217562913895</v>
+        <v>0.1523325443267822</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1256,7 +1256,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="2">
-        <v>0.06089894846081734</v>
+        <v>0.06410418450832367</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1267,7 +1267,7 @@
         <v>17</v>
       </c>
       <c r="C80" s="2">
-        <v>0.01156466081738472</v>
+        <v>0.01528874039649963</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1278,7 +1278,7 @@
         <v>18</v>
       </c>
       <c r="C81" s="2">
-        <v>0.001556041883304715</v>
+        <v>0.001537438482046127</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1289,7 +1289,7 @@
         <v>19</v>
       </c>
       <c r="C82" s="2">
-        <v>0.001583805540576577</v>
+        <v>0.001537438482046127</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1300,7 +1300,7 @@
         <v>20</v>
       </c>
       <c r="C83" s="2">
-        <v>0.001583805540576577</v>
+        <v>0.00151723250746727</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1311,7 +1311,7 @@
         <v>21</v>
       </c>
       <c r="C84" s="2">
-        <v>0.001501603168435395</v>
+        <v>0.001435030368156731</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1322,7 +1322,7 @@
         <v>22</v>
       </c>
       <c r="C85" s="2">
-        <v>0.001563654048368335</v>
+        <v>0.001435030368156731</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1333,7 +1333,7 @@
         <v>23</v>
       </c>
       <c r="C86" s="2">
-        <v>0.001568500185385346</v>
+        <v>0.001428183633834124</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="2">
-        <v>0.001733636716380715</v>
+        <v>0.001704448601230979</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="2">
-        <v>0.001733636716380715</v>
+        <v>0.001704448601230979</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1366,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="C89" s="2">
-        <v>0.001756184617988765</v>
+        <v>0.001694340142421424</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1377,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="2">
-        <v>0.001756184617988765</v>
+        <v>0.001689968397840858</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1388,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="C91" s="2">
-        <v>0.001756184617988765</v>
+        <v>0.001689968397840858</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1399,7 +1399,7 @@
         <v>5</v>
       </c>
       <c r="C92" s="2">
-        <v>0.01143230218440294</v>
+        <v>0.01330376043915749</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1410,7 +1410,7 @@
         <v>6</v>
       </c>
       <c r="C93" s="2">
-        <v>0.0287928469479084</v>
+        <v>0.06405171006917953</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1421,7 +1421,7 @@
         <v>7</v>
       </c>
       <c r="C94" s="2">
-        <v>0.08219009637832642</v>
+        <v>0.1647649109363556</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1432,7 +1432,7 @@
         <v>8</v>
       </c>
       <c r="C95" s="2">
-        <v>0.1286930292844772</v>
+        <v>0.3179423809051514</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1443,7 +1443,7 @@
         <v>9</v>
       </c>
       <c r="C96" s="2">
-        <v>0.1975026726722717</v>
+        <v>0.3953341543674469</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1454,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="C97" s="2">
-        <v>0.2555395662784576</v>
+        <v>0.5063643455505371</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1465,7 +1465,7 @@
         <v>11</v>
       </c>
       <c r="C98" s="2">
-        <v>0.2725025713443756</v>
+        <v>0.5214986205101013</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1476,7 +1476,7 @@
         <v>12</v>
       </c>
       <c r="C99" s="2">
-        <v>0.2647063434123993</v>
+        <v>0.4125715494155884</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1487,7 +1487,7 @@
         <v>13</v>
       </c>
       <c r="C100" s="2">
-        <v>0.2649151086807251</v>
+        <v>0.3991870284080505</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1498,7 +1498,7 @@
         <v>14</v>
       </c>
       <c r="C101" s="2">
-        <v>0.1987317353487015</v>
+        <v>0.297079861164093</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1509,7 +1509,7 @@
         <v>15</v>
       </c>
       <c r="C102" s="2">
-        <v>0.1149248257279396</v>
+        <v>0.175344780087471</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1520,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="2">
-        <v>0.05659082159399986</v>
+        <v>0.0644887238740921</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1531,7 +1531,7 @@
         <v>17</v>
       </c>
       <c r="C104" s="2">
-        <v>0.009635308757424355</v>
+        <v>0.01388422586023808</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1542,7 +1542,7 @@
         <v>18</v>
       </c>
       <c r="C105" s="2">
-        <v>0.001647861674427986</v>
+        <v>0.001580415526404977</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1553,7 +1553,7 @@
         <v>19</v>
       </c>
       <c r="C106" s="2">
-        <v>0.001537438482046127</v>
+        <v>0.001585810794495046</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1564,7 +1564,7 @@
         <v>20</v>
       </c>
       <c r="C107" s="2">
-        <v>0.00151723250746727</v>
+        <v>0.001585810794495046</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1575,7 +1575,7 @@
         <v>21</v>
       </c>
       <c r="C108" s="2">
-        <v>0.001435030368156731</v>
+        <v>0.001565659185871482</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1586,7 +1586,7 @@
         <v>22</v>
       </c>
       <c r="C109" s="2">
-        <v>0.001428183633834124</v>
+        <v>0.001565659185871482</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1597,7 +1597,7 @@
         <v>23</v>
       </c>
       <c r="C110" s="2">
-        <v>0.001428183633834124</v>
+        <v>0.001565659185871482</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="2">
-        <v>0.001704448601230979</v>
+        <v>0.001758344937115908</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1619,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="C112" s="2">
-        <v>0.001704448601230979</v>
+        <v>0.001757520250976086</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1630,7 +1630,7 @@
         <v>2</v>
       </c>
       <c r="C113" s="2">
-        <v>0.001694340142421424</v>
+        <v>0.001823237049393356</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1641,7 +1641,7 @@
         <v>3</v>
       </c>
       <c r="C114" s="2">
-        <v>0.001694340142421424</v>
+        <v>0.001841441029682755</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1652,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="C115" s="2">
-        <v>0.001700077555142343</v>
+        <v>0.001865287078544497</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1663,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="C116" s="2">
-        <v>0.01190492697060108</v>
+        <v>0.009540540166199207</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1674,7 +1674,7 @@
         <v>6</v>
       </c>
       <c r="C117" s="2">
-        <v>0.05546683445572853</v>
+        <v>0.02948394045233727</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1685,7 +1685,7 @@
         <v>7</v>
       </c>
       <c r="C118" s="2">
-        <v>0.1654088199138641</v>
+        <v>0.07718181610107422</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1696,7 +1696,7 @@
         <v>8</v>
       </c>
       <c r="C119" s="2">
-        <v>0.3179423809051514</v>
+        <v>0.1604147702455521</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1707,7 +1707,7 @@
         <v>9</v>
       </c>
       <c r="C120" s="2">
-        <v>0.3798587024211884</v>
+        <v>0.2611837387084961</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1718,7 +1718,7 @@
         <v>10</v>
       </c>
       <c r="C121" s="2">
-        <v>0.5063643455505371</v>
+        <v>0.3101291060447693</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1729,7 +1729,7 @@
         <v>11</v>
       </c>
       <c r="C122" s="2">
-        <v>0.5315657258033752</v>
+        <v>0.3966013193130493</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1740,7 +1740,7 @@
         <v>12</v>
       </c>
       <c r="C123" s="2">
-        <v>0.5564085841178894</v>
+        <v>0.3047942519187927</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1751,7 +1751,7 @@
         <v>13</v>
       </c>
       <c r="C124" s="2">
-        <v>0.4304633736610413</v>
+        <v>0.2757074534893036</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1762,7 +1762,7 @@
         <v>14</v>
       </c>
       <c r="C125" s="2">
-        <v>0.2709257900714874</v>
+        <v>0.2165765911340714</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1773,7 +1773,7 @@
         <v>15</v>
       </c>
       <c r="C126" s="2">
-        <v>0.1721682399511337</v>
+        <v>0.1215275973081589</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1784,7 +1784,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="2">
-        <v>0.06137294322252274</v>
+        <v>0.06067312508821487</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1795,7 +1795,7 @@
         <v>17</v>
       </c>
       <c r="C128" s="2">
-        <v>0.01154058333486319</v>
+        <v>0.01153775025159121</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1806,7 +1806,7 @@
         <v>18</v>
       </c>
       <c r="C129" s="2">
-        <v>0.00157685112208128</v>
+        <v>0.001605202909559011</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1817,7 +1817,7 @@
         <v>19</v>
       </c>
       <c r="C130" s="2">
-        <v>0.001580415526404977</v>
+        <v>0.001605202909559011</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1828,7 +1828,7 @@
         <v>20</v>
       </c>
       <c r="C131" s="2">
-        <v>0.001580415526404977</v>
+        <v>0.001501133199781179</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1839,7 +1839,7 @@
         <v>21</v>
       </c>
       <c r="C132" s="2">
-        <v>0.001503608305938542</v>
+        <v>0.001418930711224675</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1850,7 +1850,7 @@
         <v>22</v>
       </c>
       <c r="C133" s="2">
-        <v>0.001503608305938542</v>
+        <v>0.001389987068250775</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="C134" s="2">
-        <v>0.001503608305938542</v>
+        <v>0.001485339133068919</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1872,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="C135" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.001801040023565292</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1883,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.001801040023565292</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1894,7 +1894,7 @@
         <v>2</v>
       </c>
       <c r="C137" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.001747380709275603</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1905,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="C138" s="2">
-        <v>0.001820396166294813</v>
+        <v>0.001752226846292615</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -1916,7 +1916,7 @@
         <v>4</v>
       </c>
       <c r="C139" s="2">
-        <v>0.001820396166294813</v>
+        <v>0.001752226846292615</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -1927,7 +1927,7 @@
         <v>5</v>
       </c>
       <c r="C140" s="2">
-        <v>0.009434782899916172</v>
+        <v>0.008160963654518127</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1938,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="C141" s="2">
-        <v>0.03046689368784428</v>
+        <v>0.03705177083611488</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -1949,7 +1949,7 @@
         <v>7</v>
       </c>
       <c r="C142" s="2">
-        <v>0.08427612483501434</v>
+        <v>0.1003308445215225</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -1960,7 +1960,7 @@
         <v>8</v>
       </c>
       <c r="C143" s="2">
-        <v>0.2243581712245941</v>
+        <v>0.1671860218048096</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -1971,7 +1971,7 @@
         <v>9</v>
       </c>
       <c r="C144" s="2">
-        <v>0.2947062849998474</v>
+        <v>0.237297847867012</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -1982,7 +1982,7 @@
         <v>10</v>
       </c>
       <c r="C145" s="2">
-        <v>0.4328055679798126</v>
+        <v>0.3366087675094604</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -1993,7 +1993,7 @@
         <v>11</v>
       </c>
       <c r="C146" s="2">
-        <v>0.5422999858856201</v>
+        <v>0.3230690360069275</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2004,7 +2004,7 @@
         <v>12</v>
       </c>
       <c r="C147" s="2">
-        <v>0.4908904731273651</v>
+        <v>0.2860280275344849</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2015,7 +2015,7 @@
         <v>13</v>
       </c>
       <c r="C148" s="2">
-        <v>0.3367727398872375</v>
+        <v>0.2381410598754883</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2026,7 +2026,7 @@
         <v>14</v>
       </c>
       <c r="C149" s="2">
-        <v>0.2858901917934418</v>
+        <v>0.1884778290987015</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2037,7 +2037,7 @@
         <v>15</v>
       </c>
       <c r="C150" s="2">
-        <v>0.1880656629800797</v>
+        <v>0.1038088798522949</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2048,7 +2048,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="2">
-        <v>0.06319338828325272</v>
+        <v>0.04213431105017662</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2059,7 +2059,7 @@
         <v>17</v>
       </c>
       <c r="C152" s="2">
-        <v>0.01380932703614235</v>
+        <v>0.008502485230565071</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2070,7 +2070,7 @@
         <v>18</v>
       </c>
       <c r="C153" s="2">
-        <v>0.001597310299985111</v>
+        <v>0.001546897459775209</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2081,7 +2081,7 @@
         <v>19</v>
       </c>
       <c r="C154" s="2">
-        <v>0.00157685112208128</v>
+        <v>0.001628369558602571</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2092,7 +2092,7 @@
         <v>20</v>
       </c>
       <c r="C155" s="2">
-        <v>0.00157685112208128</v>
+        <v>0.001608869526535273</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2103,7 +2103,7 @@
         <v>21</v>
       </c>
       <c r="C156" s="2">
-        <v>0.001494648749940097</v>
+        <v>0.001526666805148125</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2114,7 +2114,7 @@
         <v>22</v>
       </c>
       <c r="C157" s="2">
-        <v>0.001497388002462685</v>
+        <v>0.001417750725522637</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2125,7 +2125,7 @@
         <v>23</v>
       </c>
       <c r="C158" s="2">
-        <v>0.001497388002462685</v>
+        <v>0.001417750725522637</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="C159" s="2">
-        <v>0.00172857625875622</v>
+        <v>0.001733452081680298</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="C160" s="2">
-        <v>0.00172857625875622</v>
+        <v>0.001733452081680298</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2158,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="C161" s="2">
-        <v>0.001757520250976086</v>
+        <v>0.001801040023565292</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2169,7 +2169,7 @@
         <v>3</v>
       </c>
       <c r="C162" s="2">
-        <v>0.001757520250976086</v>
+        <v>0.00183080870192498</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2180,7 +2180,7 @@
         <v>4</v>
       </c>
       <c r="C163" s="2">
-        <v>0.001757520250976086</v>
+        <v>0.001749385381117463</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2191,7 +2191,7 @@
         <v>5</v>
       </c>
       <c r="C164" s="2">
-        <v>0.009094623848795891</v>
+        <v>0.01327463705092669</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2202,7 +2202,7 @@
         <v>6</v>
       </c>
       <c r="C165" s="2">
-        <v>0.04337866604328156</v>
+        <v>0.03830048441886902</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2213,7 +2213,7 @@
         <v>7</v>
       </c>
       <c r="C166" s="2">
-        <v>0.09367484599351883</v>
+        <v>0.1215591877698898</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2224,7 +2224,7 @@
         <v>8</v>
       </c>
       <c r="C167" s="2">
-        <v>0.2228189557790756</v>
+        <v>0.2096128314733505</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2235,7 +2235,7 @@
         <v>9</v>
       </c>
       <c r="C168" s="2">
-        <v>0.2853198051452637</v>
+        <v>0.2917116582393646</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2246,7 +2246,7 @@
         <v>10</v>
       </c>
       <c r="C169" s="2">
-        <v>0.3667512536048889</v>
+        <v>0.3016287982463837</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2257,7 +2257,7 @@
         <v>11</v>
       </c>
       <c r="C170" s="2">
-        <v>0.3327758014202118</v>
+        <v>0.3617633879184723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the Dates and Intervals to the Solina Consumption Predictions file.
</commit_message>
<xml_diff>
--- a/Solina/Production/Results_Production_xgb.xlsx
+++ b/Solina/Production/Results_Production_xgb.xlsx
@@ -25,18 +25,6 @@
     <t>Prediction</t>
   </si>
   <si>
-    <t>2024-03-22</t>
-  </si>
-  <si>
-    <t>2024-03-23</t>
-  </si>
-  <si>
-    <t>2024-03-24</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
     <t>2024-03-26</t>
   </si>
   <si>
@@ -47,6 +35,18 @@
   </si>
   <si>
     <t>2024-03-29</t>
+  </si>
+  <si>
+    <t>2024-03-30</t>
+  </si>
+  <si>
+    <t>2024-03-31</t>
+  </si>
+  <si>
+    <t>2024-04-01</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
   </si>
 </sst>
 </file>
@@ -406,10 +406,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
-        <v>0.531111478805542</v>
+        <v>0.09700000286102295</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -417,10 +417,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
-        <v>0.5527240633964539</v>
+        <v>0.01799999922513962</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
-        <v>0.4280891418457031</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -439,10 +439,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
-        <v>0.2591042816638947</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -450,10 +450,10 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
-        <v>0.1504656076431274</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -461,10 +461,10 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
-        <v>0.06011993438005447</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -472,10 +472,10 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2">
-        <v>0.009618937037885189</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -483,65 +483,65 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
-        <v>0.001596485148184001</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>0.001596485148184001</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>0.00157602597028017</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2">
-        <v>0.001498213154263794</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="B13">
-        <v>22</v>
-      </c>
       <c r="C13" s="2">
-        <v>0.001498213154263794</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>0.001498213154263794</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -549,10 +549,10 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.008999999612569809</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -560,10 +560,10 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.04600000008940697</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -571,10 +571,10 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.1420000046491623</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -582,10 +582,10 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2">
-        <v>0.001820396166294813</v>
+        <v>0.164000004529953</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -593,10 +593,10 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2">
-        <v>0.001820396166294813</v>
+        <v>0.2790000140666962</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -604,10 +604,10 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2">
-        <v>0.009711515158414841</v>
+        <v>0.3199999928474426</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -615,10 +615,10 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2">
-        <v>0.03872333094477654</v>
+        <v>0.3519999980926514</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -626,10 +626,10 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2">
-        <v>0.1275391280651093</v>
+        <v>0.3030000030994415</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -637,10 +637,10 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2">
-        <v>0.3109587728977203</v>
+        <v>0.257999986410141</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -648,10 +648,10 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2">
-        <v>0.3965180814266205</v>
+        <v>0.2680000066757202</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -659,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2">
-        <v>0.5021463632583618</v>
+        <v>0.1589999943971634</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -670,10 +670,10 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2">
-        <v>0.5473080277442932</v>
+        <v>0.06100000068545341</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -681,10 +681,10 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C27" s="2">
-        <v>0.5518757104873657</v>
+        <v>0.01200000010430813</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -692,10 +692,10 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C28" s="2">
-        <v>0.4413212239742279</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -703,10 +703,10 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C29" s="2">
-        <v>0.337122917175293</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -714,10 +714,10 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2">
-        <v>0.2171129137277603</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -725,10 +725,10 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2">
-        <v>0.08976252377033234</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -736,10 +736,10 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2">
-        <v>0.01414182223379612</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -747,65 +747,65 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2">
-        <v>0.001606028061360121</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C34" s="2">
-        <v>0.001501958351582289</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C35" s="2">
-        <v>0.001501958351582289</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C36" s="2">
-        <v>0.001419755863025784</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B37">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C37" s="2">
-        <v>0.001419755863025784</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B38">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C38" s="2">
-        <v>0.001419755863025784</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -813,10 +813,10 @@
         <v>5</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C39" s="2">
-        <v>0.001735456753522158</v>
+        <v>0.01200000010430813</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -824,10 +824,10 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C40" s="2">
-        <v>0.001735456753522158</v>
+        <v>0.02700000070035458</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -835,10 +835,10 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C41" s="2">
-        <v>0.001829984015785158</v>
+        <v>0.04199999943375587</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -846,10 +846,10 @@
         <v>5</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C42" s="2">
-        <v>0.001801040023565292</v>
+        <v>0.09099999815225601</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -857,10 +857,10 @@
         <v>5</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C43" s="2">
-        <v>0.001747380709275603</v>
+        <v>0.1449999958276749</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -868,10 +868,10 @@
         <v>5</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C44" s="2">
-        <v>0.008163020014762878</v>
+        <v>0.1829999983310699</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -879,10 +879,10 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C45" s="2">
-        <v>0.03103868290781975</v>
+        <v>0.2269999980926514</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -890,10 +890,10 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C46" s="2">
-        <v>0.08109454065561295</v>
+        <v>0.2460000067949295</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -901,10 +901,10 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C47" s="2">
-        <v>0.1491440683603287</v>
+        <v>0.2160000056028366</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -912,10 +912,10 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C48" s="2">
-        <v>0.2794862687587738</v>
+        <v>0.1969999969005585</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -923,10 +923,10 @@
         <v>5</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C49" s="2">
-        <v>0.3724546730518341</v>
+        <v>0.1180000007152557</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -934,10 +934,10 @@
         <v>5</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C50" s="2">
-        <v>0.3133758306503296</v>
+        <v>0.05900000035762787</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -945,10 +945,10 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C51" s="2">
-        <v>0.2397262752056122</v>
+        <v>0.01400000043213367</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -956,10 +956,10 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C52" s="2">
-        <v>0.1865478008985519</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -967,10 +967,10 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C53" s="2">
-        <v>0.1299076229333878</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -978,10 +978,10 @@
         <v>5</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C54" s="2">
-        <v>0.06683869659900665</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -989,10 +989,10 @@
         <v>5</v>
       </c>
       <c r="B55">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C55" s="2">
-        <v>0.03296571597456932</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1000,10 +1000,10 @@
         <v>5</v>
       </c>
       <c r="B56">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C56" s="2">
-        <v>0.01277642976492643</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1011,65 +1011,65 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C57" s="2">
-        <v>0.001582328230142593</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B58">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C58" s="2">
-        <v>0.001582328230142593</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C59" s="2">
-        <v>0.001582328230142593</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C60" s="2">
-        <v>0.001500125625170767</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C61" s="2">
-        <v>0.001479919767007232</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B62">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C62" s="2">
-        <v>0.001479919767007232</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1077,10 +1077,10 @@
         <v>6</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C63" s="2">
-        <v>0.001756184617988765</v>
+        <v>0.01400000043213367</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1088,10 +1088,10 @@
         <v>6</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C64" s="2">
-        <v>0.001756184617988765</v>
+        <v>0.06499999761581421</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1099,10 +1099,10 @@
         <v>6</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C65" s="2">
-        <v>0.001745106419548392</v>
+        <v>0.1519999951124191</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1110,10 +1110,10 @@
         <v>6</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C66" s="2">
-        <v>0.001709290081635118</v>
+        <v>0.2290000021457672</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1121,10 +1121,10 @@
         <v>6</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C67" s="2">
-        <v>0.001681526424363256</v>
+        <v>0.2849999964237213</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1132,10 +1132,10 @@
         <v>6</v>
       </c>
       <c r="B68">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2">
-        <v>0.009383793920278549</v>
+        <v>0.4129999876022339</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1143,10 +1143,10 @@
         <v>6</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C69" s="2">
-        <v>0.04251806437969208</v>
+        <v>0.4990000128746033</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1154,10 +1154,10 @@
         <v>6</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C70" s="2">
-        <v>0.1151808798313141</v>
+        <v>0.4709999859333038</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1165,10 +1165,10 @@
         <v>6</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C71" s="2">
-        <v>0.2080928087234497</v>
+        <v>0.3339999914169312</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1176,10 +1176,10 @@
         <v>6</v>
       </c>
       <c r="B72">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C72" s="2">
-        <v>0.2761012315750122</v>
+        <v>0.3289999961853027</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1187,10 +1187,10 @@
         <v>6</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C73" s="2">
-        <v>0.4675039947032928</v>
+        <v>0.2440000027418137</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1198,10 +1198,10 @@
         <v>6</v>
       </c>
       <c r="B74">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C74" s="2">
-        <v>0.4026133120059967</v>
+        <v>0.1120000034570694</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1209,10 +1209,10 @@
         <v>6</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C75" s="2">
-        <v>0.4187763035297394</v>
+        <v>0.01899999938905239</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1220,10 +1220,10 @@
         <v>6</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C76" s="2">
-        <v>0.3243970274925232</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1231,10 +1231,10 @@
         <v>6</v>
       </c>
       <c r="B77">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C77" s="2">
-        <v>0.2554626762866974</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1242,10 +1242,10 @@
         <v>6</v>
       </c>
       <c r="B78">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C78" s="2">
-        <v>0.1523325443267822</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1253,10 +1253,10 @@
         <v>6</v>
       </c>
       <c r="B79">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C79" s="2">
-        <v>0.06410418450832367</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1264,10 +1264,10 @@
         <v>6</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C80" s="2">
-        <v>0.01528874039649963</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1275,65 +1275,65 @@
         <v>6</v>
       </c>
       <c r="B81">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C81" s="2">
-        <v>0.001537438482046127</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B82">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C82" s="2">
-        <v>0.001537438482046127</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C83" s="2">
-        <v>0.00151723250746727</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B84">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C84" s="2">
-        <v>0.001435030368156731</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B85">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C85" s="2">
-        <v>0.001435030368156731</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B86">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C86" s="2">
-        <v>0.001428183633834124</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1341,10 +1341,10 @@
         <v>7</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C87" s="2">
-        <v>0.001704448601230979</v>
+        <v>0.02099999971687794</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1352,10 +1352,10 @@
         <v>7</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C88" s="2">
-        <v>0.001704448601230979</v>
+        <v>0.04800000041723251</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1363,10 +1363,10 @@
         <v>7</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C89" s="2">
-        <v>0.001694340142421424</v>
+        <v>0.1239999979734421</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1374,10 +1374,10 @@
         <v>7</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C90" s="2">
-        <v>0.001689968397840858</v>
+        <v>0.2119999974966049</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1385,10 +1385,10 @@
         <v>7</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C91" s="2">
-        <v>0.001689968397840858</v>
+        <v>0.2870000004768372</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1396,10 +1396,10 @@
         <v>7</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C92" s="2">
-        <v>0.01330376043915749</v>
+        <v>0.4120000004768372</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1407,10 +1407,10 @@
         <v>7</v>
       </c>
       <c r="B93">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C93" s="2">
-        <v>0.06405171006917953</v>
+        <v>0.4189999997615814</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1418,10 +1418,10 @@
         <v>7</v>
       </c>
       <c r="B94">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C94" s="2">
-        <v>0.1647649109363556</v>
+        <v>0.5139999985694885</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1429,10 +1429,10 @@
         <v>7</v>
       </c>
       <c r="B95">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C95" s="2">
-        <v>0.3179423809051514</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1440,10 +1440,10 @@
         <v>7</v>
       </c>
       <c r="B96">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C96" s="2">
-        <v>0.3953341543674469</v>
+        <v>0.2750000059604645</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1451,10 +1451,10 @@
         <v>7</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C97" s="2">
-        <v>0.5063643455505371</v>
+        <v>0.1720000058412552</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1462,10 +1462,10 @@
         <v>7</v>
       </c>
       <c r="B98">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C98" s="2">
-        <v>0.5214986205101013</v>
+        <v>0.05799999833106995</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1473,10 +1473,10 @@
         <v>7</v>
       </c>
       <c r="B99">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C99" s="2">
-        <v>0.4125715494155884</v>
+        <v>0.01499999966472387</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1484,10 +1484,10 @@
         <v>7</v>
       </c>
       <c r="B100">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C100" s="2">
-        <v>0.3991870284080505</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1495,10 +1495,10 @@
         <v>7</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C101" s="2">
-        <v>0.297079861164093</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1506,10 +1506,10 @@
         <v>7</v>
       </c>
       <c r="B102">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C102" s="2">
-        <v>0.175344780087471</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1517,10 +1517,10 @@
         <v>7</v>
       </c>
       <c r="B103">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C103" s="2">
-        <v>0.0644887238740921</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1528,10 +1528,10 @@
         <v>7</v>
       </c>
       <c r="B104">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C104" s="2">
-        <v>0.01388422586023808</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1539,65 +1539,65 @@
         <v>7</v>
       </c>
       <c r="B105">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C105" s="2">
-        <v>0.001580415526404977</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B106">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C106" s="2">
-        <v>0.001585810794495046</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C107" s="2">
-        <v>0.001585810794495046</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B108">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C108" s="2">
-        <v>0.001565659185871482</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B109">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C109" s="2">
-        <v>0.001565659185871482</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B110">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C110" s="2">
-        <v>0.001565659185871482</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1605,10 +1605,10 @@
         <v>8</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C111" s="2">
-        <v>0.001758344937115908</v>
+        <v>0.01999999955296516</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1616,10 +1616,10 @@
         <v>8</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C112" s="2">
-        <v>0.001757520250976086</v>
+        <v>0.06800000369548798</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1627,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C113" s="2">
-        <v>0.001823237049393356</v>
+        <v>0.153999999165535</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1638,10 +1638,10 @@
         <v>8</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C114" s="2">
-        <v>0.001841441029682755</v>
+        <v>0.2829999923706055</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1649,10 +1649,10 @@
         <v>8</v>
       </c>
       <c r="B115">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C115" s="2">
-        <v>0.001865287078544497</v>
+        <v>0.2720000147819519</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1660,10 +1660,10 @@
         <v>8</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C116" s="2">
-        <v>0.009540540166199207</v>
+        <v>0.3700000047683716</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1671,10 +1671,10 @@
         <v>8</v>
       </c>
       <c r="B117">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C117" s="2">
-        <v>0.02948394045233727</v>
+        <v>0.453000009059906</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1682,10 +1682,10 @@
         <v>8</v>
       </c>
       <c r="B118">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C118" s="2">
-        <v>0.07718181610107422</v>
+        <v>0.4850000143051147</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1693,10 +1693,10 @@
         <v>8</v>
       </c>
       <c r="B119">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C119" s="2">
-        <v>0.1604147702455521</v>
+        <v>0.4199999868869781</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1704,10 +1704,10 @@
         <v>8</v>
       </c>
       <c r="B120">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C120" s="2">
-        <v>0.2611837387084961</v>
+        <v>0.3449999988079071</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1715,10 +1715,10 @@
         <v>8</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C121" s="2">
-        <v>0.3101291060447693</v>
+        <v>0.1979999989271164</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1726,10 +1726,10 @@
         <v>8</v>
       </c>
       <c r="B122">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C122" s="2">
-        <v>0.3966013193130493</v>
+        <v>0.1129999980330467</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1737,10 +1737,10 @@
         <v>8</v>
       </c>
       <c r="B123">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C123" s="2">
-        <v>0.3047942519187927</v>
+        <v>0.01799999922513962</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1748,10 +1748,10 @@
         <v>8</v>
       </c>
       <c r="B124">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C124" s="2">
-        <v>0.2757074534893036</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1759,10 +1759,10 @@
         <v>8</v>
       </c>
       <c r="B125">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C125" s="2">
-        <v>0.2165765911340714</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1770,10 +1770,10 @@
         <v>8</v>
       </c>
       <c r="B126">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C126" s="2">
-        <v>0.1215275973081589</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1781,10 +1781,10 @@
         <v>8</v>
       </c>
       <c r="B127">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C127" s="2">
-        <v>0.06067312508821487</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1792,10 +1792,10 @@
         <v>8</v>
       </c>
       <c r="B128">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C128" s="2">
-        <v>0.01153775025159121</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1803,65 +1803,65 @@
         <v>8</v>
       </c>
       <c r="B129">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C129" s="2">
-        <v>0.001605202909559011</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B130">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C130" s="2">
-        <v>0.001605202909559011</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B131">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C131" s="2">
-        <v>0.001501133199781179</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B132">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C132" s="2">
-        <v>0.001418930711224675</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B133">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C133" s="2">
-        <v>0.001389987068250775</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B134">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C134" s="2">
-        <v>0.001485339133068919</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1869,10 +1869,10 @@
         <v>9</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C135" s="2">
-        <v>0.001801040023565292</v>
+        <v>0.01799999922513962</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1880,10 +1880,10 @@
         <v>9</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C136" s="2">
-        <v>0.001801040023565292</v>
+        <v>0.06800000369548798</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1891,10 +1891,10 @@
         <v>9</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C137" s="2">
-        <v>0.001747380709275603</v>
+        <v>0.1920000016689301</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1902,10 +1902,10 @@
         <v>9</v>
       </c>
       <c r="B138">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C138" s="2">
-        <v>0.001752226846292615</v>
+        <v>0.2840000092983246</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -1913,10 +1913,10 @@
         <v>9</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C139" s="2">
-        <v>0.001752226846292615</v>
+        <v>0.2899999916553497</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -1924,10 +1924,10 @@
         <v>9</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C140" s="2">
-        <v>0.008160963654518127</v>
+        <v>0.4210000038146973</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1935,10 +1935,10 @@
         <v>9</v>
       </c>
       <c r="B141">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C141" s="2">
-        <v>0.03705177083611488</v>
+        <v>0.4650000035762787</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -1946,10 +1946,10 @@
         <v>9</v>
       </c>
       <c r="B142">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C142" s="2">
-        <v>0.1003308445215225</v>
+        <v>0.5040000081062317</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -1957,10 +1957,10 @@
         <v>9</v>
       </c>
       <c r="B143">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C143" s="2">
-        <v>0.1671860218048096</v>
+        <v>0.5040000081062317</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -1968,10 +1968,10 @@
         <v>9</v>
       </c>
       <c r="B144">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C144" s="2">
-        <v>0.237297847867012</v>
+        <v>0.4149999916553497</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -1979,10 +1979,10 @@
         <v>9</v>
       </c>
       <c r="B145">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C145" s="2">
-        <v>0.3366087675094604</v>
+        <v>0.289000004529953</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -1990,10 +1990,10 @@
         <v>9</v>
       </c>
       <c r="B146">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C146" s="2">
-        <v>0.3230690360069275</v>
+        <v>0.1480000019073486</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2001,10 +2001,10 @@
         <v>9</v>
       </c>
       <c r="B147">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C147" s="2">
-        <v>0.2860280275344849</v>
+        <v>0.02899999916553497</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2012,10 +2012,10 @@
         <v>9</v>
       </c>
       <c r="B148">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C148" s="2">
-        <v>0.2381410598754883</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2023,10 +2023,10 @@
         <v>9</v>
       </c>
       <c r="B149">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C149" s="2">
-        <v>0.1884778290987015</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2034,10 +2034,10 @@
         <v>9</v>
       </c>
       <c r="B150">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C150" s="2">
-        <v>0.1038088798522949</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2045,10 +2045,10 @@
         <v>9</v>
       </c>
       <c r="B151">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C151" s="2">
-        <v>0.04213431105017662</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2056,10 +2056,10 @@
         <v>9</v>
       </c>
       <c r="B152">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C152" s="2">
-        <v>0.008502485230565071</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2067,65 +2067,65 @@
         <v>9</v>
       </c>
       <c r="B153">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C153" s="2">
-        <v>0.001546897459775209</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B154">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C154" s="2">
-        <v>0.001628369558602571</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B155">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C155" s="2">
-        <v>0.001608869526535273</v>
+        <v>0.001000000047497451</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B156">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C156" s="2">
-        <v>0.001526666805148125</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B157">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C157" s="2">
-        <v>0.001417750725522637</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C158" s="2">
-        <v>0.001417750725522637</v>
+        <v>0.002000000094994903</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2133,10 +2133,10 @@
         <v>10</v>
       </c>
       <c r="B159">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C159" s="2">
-        <v>0.001733452081680298</v>
+        <v>0.01200000010430813</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2144,10 +2144,10 @@
         <v>10</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C160" s="2">
-        <v>0.001733452081680298</v>
+        <v>0.04600000008940697</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2155,10 +2155,10 @@
         <v>10</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C161" s="2">
-        <v>0.001801040023565292</v>
+        <v>0.0989999994635582</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2166,10 +2166,10 @@
         <v>10</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C162" s="2">
-        <v>0.00183080870192498</v>
+        <v>0.1940000057220459</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2177,10 +2177,10 @@
         <v>10</v>
       </c>
       <c r="B163">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C163" s="2">
-        <v>0.001749385381117463</v>
+        <v>0.2829999923706055</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2188,10 +2188,10 @@
         <v>10</v>
       </c>
       <c r="B164">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C164" s="2">
-        <v>0.01327463705092669</v>
+        <v>0.363999992609024</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2199,10 +2199,10 @@
         <v>10</v>
       </c>
       <c r="B165">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C165" s="2">
-        <v>0.03830048441886902</v>
+        <v>0.3770000040531158</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2210,10 +2210,10 @@
         <v>10</v>
       </c>
       <c r="B166">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C166" s="2">
-        <v>0.1215591877698898</v>
+        <v>0.414000004529953</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2221,10 +2221,10 @@
         <v>10</v>
       </c>
       <c r="B167">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C167" s="2">
-        <v>0.2096128314733505</v>
+        <v>0.3549999892711639</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2232,10 +2232,10 @@
         <v>10</v>
       </c>
       <c r="B168">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C168" s="2">
-        <v>0.2917116582393646</v>
+        <v>0.3129999935626984</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2243,10 +2243,10 @@
         <v>10</v>
       </c>
       <c r="B169">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C169" s="2">
-        <v>0.3016287982463837</v>
+        <v>0.257999986410141</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2254,10 +2254,10 @@
         <v>10</v>
       </c>
       <c r="B170">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C170" s="2">
-        <v>0.3617633879184723</v>
+        <v>0.119999997317791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusting to EET the values for RAAL and Solina production data
</commit_message>
<xml_diff>
--- a/Solina/Production/Results_Production_xgb.xlsx
+++ b/Solina/Production/Results_Production_xgb.xlsx
@@ -445,59 +445,59 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>16</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.097</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.018</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>18</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -510,7 +510,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -523,7 +523,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -536,7 +536,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2024-03-26</t>
+          <t>2024-04-03</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -549,7 +549,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -562,7 +562,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -575,7 +575,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -588,7 +588,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -601,7 +601,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -614,7 +614,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -627,189 +627,189 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>6</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>7</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.142</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>8</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.164</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>9</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.279</v>
+        <v>0.117</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>10</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.32</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>11</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.352</v>
+        <v>0.271</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.303</v>
+        <v>0.305</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>13</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.258</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>14</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.268</v>
+        <v>0.319</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>15</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.159</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>16</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.061</v>
+        <v>0.241</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>17</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.012</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>18</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>19</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -822,7 +822,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -835,7 +835,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -848,7 +848,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>2024-03-27</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -861,7 +861,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -874,7 +874,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -887,7 +887,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -900,7 +900,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -913,7 +913,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -926,202 +926,202 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>0.012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>6</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>0.027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>7</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>0.042</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>8</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>0.091</v>
+        <v>0.061</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>9</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>0.145</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>10</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>0.183</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>11</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>0.227</v>
+        <v>0.345</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>12</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>0.246</v>
+        <v>0.404</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>13</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>0.216</v>
+        <v>0.411</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>14</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>0.197</v>
+        <v>0.417</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>15</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>0.118</v>
+        <v>0.356</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>16</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0.059</v>
+        <v>0.287</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>17</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>0.014</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>18</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>0</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>19</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>0</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1134,7 +1134,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1147,7 +1147,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1160,7 +1160,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>2024-03-28</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1173,7 +1173,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1186,7 +1186,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1199,7 +1199,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1212,7 +1212,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1225,7 +1225,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1238,202 +1238,202 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>5</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>0.014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>6</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>0.065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>7</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>0.152</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B66" t="n">
         <v>8</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>0.229</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>9</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>0.285</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B68" t="n">
         <v>10</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>0.413</v>
+        <v>0.352</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B69" t="n">
         <v>11</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>0.499</v>
+        <v>0.476</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>12</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>0.471</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>13</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>0.334</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B72" t="n">
         <v>14</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>0.329</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B73" t="n">
         <v>15</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>0.244</v>
+        <v>0.404</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B74" t="n">
         <v>16</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>0.112</v>
+        <v>0.283</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B75" t="n">
         <v>17</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>0.019</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B76" t="n">
         <v>18</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>0</v>
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B77" t="n">
         <v>19</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>0</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1446,7 +1446,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1459,7 +1459,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1472,7 +1472,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1485,7 +1485,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1498,7 +1498,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1511,7 +1511,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1524,7 +1524,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1537,7 +1537,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1550,202 +1550,202 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B87" t="n">
         <v>5</v>
       </c>
       <c r="C87" s="2" t="n">
-        <v>0.021</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B88" t="n">
         <v>6</v>
       </c>
       <c r="C88" s="2" t="n">
-        <v>0.048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B89" t="n">
         <v>7</v>
       </c>
       <c r="C89" s="2" t="n">
-        <v>0.124</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B90" t="n">
         <v>8</v>
       </c>
       <c r="C90" s="2" t="n">
-        <v>0.212</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B91" t="n">
         <v>9</v>
       </c>
       <c r="C91" s="2" t="n">
-        <v>0.287</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B92" t="n">
         <v>10</v>
       </c>
       <c r="C92" s="2" t="n">
-        <v>0.412</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>11</v>
       </c>
       <c r="C93" s="2" t="n">
-        <v>0.419</v>
+        <v>0.483</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>12</v>
       </c>
       <c r="C94" s="2" t="n">
-        <v>0.514</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>13</v>
       </c>
       <c r="C95" s="2" t="n">
-        <v>0.375</v>
+        <v>0.5580000000000001</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B96" t="n">
         <v>14</v>
       </c>
       <c r="C96" s="2" t="n">
-        <v>0.275</v>
+        <v>0.531</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>15</v>
       </c>
       <c r="C97" s="2" t="n">
-        <v>0.172</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>16</v>
       </c>
       <c r="C98" s="2" t="n">
-        <v>0.058</v>
+        <v>0.346</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B99" t="n">
         <v>17</v>
       </c>
       <c r="C99" s="2" t="n">
-        <v>0.015</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B100" t="n">
         <v>18</v>
       </c>
       <c r="C100" s="2" t="n">
-        <v>0</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B101" t="n">
         <v>19</v>
       </c>
       <c r="C101" s="2" t="n">
-        <v>0</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -1758,7 +1758,7 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -1771,7 +1771,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -1784,7 +1784,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>2024-03-30</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -1797,7 +1797,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -1810,7 +1810,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -1823,7 +1823,7 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -1836,7 +1836,7 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -1849,7 +1849,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -1862,202 +1862,202 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B111" t="n">
         <v>5</v>
       </c>
       <c r="C111" s="2" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B112" t="n">
         <v>6</v>
       </c>
       <c r="C112" s="2" t="n">
-        <v>0.068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B113" t="n">
         <v>7</v>
       </c>
       <c r="C113" s="2" t="n">
-        <v>0.154</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B114" t="n">
         <v>8</v>
       </c>
       <c r="C114" s="2" t="n">
-        <v>0.283</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B115" t="n">
         <v>9</v>
       </c>
       <c r="C115" s="2" t="n">
-        <v>0.272</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B116" t="n">
         <v>10</v>
       </c>
       <c r="C116" s="2" t="n">
-        <v>0.37</v>
+        <v>0.376</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B117" t="n">
         <v>11</v>
       </c>
       <c r="C117" s="2" t="n">
-        <v>0.453</v>
+        <v>0.488</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B118" t="n">
         <v>12</v>
       </c>
       <c r="C118" s="2" t="n">
-        <v>0.485</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B119" t="n">
         <v>13</v>
       </c>
       <c r="C119" s="2" t="n">
-        <v>0.42</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B120" t="n">
         <v>14</v>
       </c>
       <c r="C120" s="2" t="n">
-        <v>0.345</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B121" t="n">
         <v>15</v>
       </c>
       <c r="C121" s="2" t="n">
-        <v>0.198</v>
+        <v>0.512</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B122" t="n">
         <v>16</v>
       </c>
       <c r="C122" s="2" t="n">
-        <v>0.113</v>
+        <v>0.416</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B123" t="n">
         <v>17</v>
       </c>
       <c r="C123" s="2" t="n">
-        <v>0.018</v>
+        <v>0.303</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B124" t="n">
         <v>18</v>
       </c>
       <c r="C124" s="2" t="n">
-        <v>0</v>
+        <v>0.159</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B125" t="n">
         <v>19</v>
       </c>
       <c r="C125" s="2" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -2070,7 +2070,7 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -2083,7 +2083,7 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -2096,7 +2096,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>2024-03-31</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -2109,7 +2109,7 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -2122,7 +2122,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -2135,7 +2135,7 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -2148,7 +2148,7 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -2161,7 +2161,7 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -2174,202 +2174,202 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B135" t="n">
         <v>5</v>
       </c>
       <c r="C135" s="2" t="n">
-        <v>0.018</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B136" t="n">
         <v>6</v>
       </c>
       <c r="C136" s="2" t="n">
-        <v>0.068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B137" t="n">
         <v>7</v>
       </c>
       <c r="C137" s="2" t="n">
-        <v>0.192</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B138" t="n">
         <v>8</v>
       </c>
       <c r="C138" s="2" t="n">
-        <v>0.284</v>
+        <v>0.116</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B139" t="n">
         <v>9</v>
       </c>
       <c r="C139" s="2" t="n">
-        <v>0.29</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B140" t="n">
         <v>10</v>
       </c>
       <c r="C140" s="2" t="n">
-        <v>0.421</v>
+        <v>0.383</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B141" t="n">
         <v>11</v>
       </c>
       <c r="C141" s="2" t="n">
-        <v>0.465</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B142" t="n">
         <v>12</v>
       </c>
       <c r="C142" s="2" t="n">
-        <v>0.504</v>
+        <v>0.552</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B143" t="n">
         <v>13</v>
       </c>
       <c r="C143" s="2" t="n">
-        <v>0.504</v>
+        <v>0.5639999999999999</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B144" t="n">
         <v>14</v>
       </c>
       <c r="C144" s="2" t="n">
-        <v>0.415</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B145" t="n">
         <v>15</v>
       </c>
       <c r="C145" s="2" t="n">
-        <v>0.289</v>
+        <v>0.486</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B146" t="n">
         <v>16</v>
       </c>
       <c r="C146" s="2" t="n">
-        <v>0.148</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B147" t="n">
         <v>17</v>
       </c>
       <c r="C147" s="2" t="n">
-        <v>0.029</v>
+        <v>0.274</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B148" t="n">
         <v>18</v>
       </c>
       <c r="C148" s="2" t="n">
-        <v>0</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B149" t="n">
         <v>19</v>
       </c>
       <c r="C149" s="2" t="n">
-        <v>0</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -2382,7 +2382,7 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -2395,7 +2395,7 @@
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -2408,7 +2408,7 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -2421,7 +2421,7 @@
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -2434,7 +2434,7 @@
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -2447,7 +2447,7 @@
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -2460,7 +2460,7 @@
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -2473,7 +2473,7 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -2486,157 +2486,157 @@
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B159" t="n">
         <v>5</v>
       </c>
       <c r="C159" s="2" t="n">
-        <v>0.012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B160" t="n">
         <v>6</v>
       </c>
       <c r="C160" s="2" t="n">
-        <v>0.046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B161" t="n">
         <v>7</v>
       </c>
       <c r="C161" s="2" t="n">
-        <v>0.099</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B162" t="n">
         <v>8</v>
       </c>
       <c r="C162" s="2" t="n">
-        <v>0.194</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B163" t="n">
         <v>9</v>
       </c>
       <c r="C163" s="2" t="n">
-        <v>0.283</v>
+        <v>0.268</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B164" t="n">
         <v>10</v>
       </c>
       <c r="C164" s="2" t="n">
-        <v>0.364</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B165" t="n">
         <v>11</v>
       </c>
       <c r="C165" s="2" t="n">
-        <v>0.377</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B166" t="n">
         <v>12</v>
       </c>
       <c r="C166" s="2" t="n">
-        <v>0.414</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B167" t="n">
         <v>13</v>
       </c>
       <c r="C167" s="2" t="n">
-        <v>0.355</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B168" t="n">
         <v>14</v>
       </c>
       <c r="C168" s="2" t="n">
-        <v>0.313</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B169" t="n">
         <v>15</v>
       </c>
       <c r="C169" s="2" t="n">
-        <v>0.258</v>
+        <v>0.499</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B170" t="n">
         <v>16</v>
       </c>
       <c r="C170" s="2" t="n">
-        <v>0.12</v>
+        <v>0.379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the requirements.txt withwapi
</commit_message>
<xml_diff>
--- a/Solina/Production/Results_Production_xgb.xlsx
+++ b/Solina/Production/Results_Production_xgb.xlsx
@@ -445,11 +445,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>0</v>
@@ -458,11 +458,11 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
@@ -471,79 +471,79 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.066</v>
+        <v>0.292</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.013</v>
+        <v>0.309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0</v>
+        <v>0.427</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0</v>
+        <v>0.303</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2024-04-03</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0</v>
+        <v>0.229</v>
       </c>
     </row>
     <row r="10">
@@ -553,10 +553,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0</v>
+        <v>0.169</v>
       </c>
     </row>
     <row r="11">
@@ -566,10 +566,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0</v>
+        <v>0.076</v>
       </c>
     </row>
     <row r="12">
@@ -579,10 +579,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="13">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>0</v>
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0</v>
@@ -631,7 +631,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
@@ -640,222 +640,222 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.326</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.319</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.307</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.241</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.185</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.082</v>
+        <v>0.262</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.016</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0</v>
+        <v>0.403</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0</v>
+        <v>0.405</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>0</v>
+        <v>0.301</v>
       </c>
     </row>
     <row r="34">
@@ -865,10 +865,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="35">
@@ -878,10 +878,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -891,10 +891,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>0</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="37">
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>0</v>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0</v>
@@ -943,7 +943,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
@@ -952,222 +952,222 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>0.014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>0.061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>0.252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>0.345</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>0.404</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>0.411</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>0.417</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>0.356</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0.287</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>0.189</v>
+        <v>0.219</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>0.083</v>
+        <v>0.284</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>0.015</v>
+        <v>0.365</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>0</v>
+        <v>0.397</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>0</v>
+        <v>0.321</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>0</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="58">
@@ -1177,10 +1177,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>0</v>
+        <v>0.146</v>
       </c>
     </row>
     <row r="59">
@@ -1190,10 +1190,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="60">
@@ -1203,10 +1203,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>0</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="61">
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>0</v>
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>0</v>
@@ -1264,222 +1264,222 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>0.015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>0.217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>0.352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>0.476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>0.525</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>0.475</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>0.404</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>0.283</v>
+        <v>0.241</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>0.193</v>
+        <v>0.359</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.515</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>0.015</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>0</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C79" s="2" t="n">
-        <v>0</v>
+        <v>0.572</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>0</v>
+        <v>0.498</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>0</v>
+        <v>0.388</v>
       </c>
     </row>
     <row r="82">
@@ -1489,10 +1489,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>0</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="83">
@@ -1502,10 +1502,10 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>0</v>
+        <v>0.139</v>
       </c>
     </row>
     <row r="84">
@@ -1515,10 +1515,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C84" s="2" t="n">
-        <v>0</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="85">
@@ -1528,7 +1528,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C86" s="2" t="n">
         <v>0</v>
@@ -1554,7 +1554,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C87" s="2" t="n">
         <v>0</v>
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>0</v>
@@ -1576,222 +1576,222 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C89" s="2" t="n">
-        <v>0.024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C90" s="2" t="n">
-        <v>0.118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C91" s="2" t="n">
-        <v>0.256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C92" s="2" t="n">
-        <v>0.385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C93" s="2" t="n">
-        <v>0.483</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C94" s="2" t="n">
-        <v>0.544</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C95" s="2" t="n">
-        <v>0.5580000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C96" s="2" t="n">
-        <v>0.531</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C97" s="2" t="n">
-        <v>0.455</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C98" s="2" t="n">
-        <v>0.346</v>
+        <v>0.262</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C99" s="2" t="n">
-        <v>0.242</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C100" s="2" t="n">
-        <v>0.124</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C101" s="2" t="n">
-        <v>0.024</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C102" s="2" t="n">
-        <v>0</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C103" s="2" t="n">
-        <v>0</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C104" s="2" t="n">
-        <v>0</v>
+        <v>0.522</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C105" s="2" t="n">
-        <v>0</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="106">
@@ -1801,10 +1801,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C106" s="2" t="n">
-        <v>0</v>
+        <v>0.297</v>
       </c>
     </row>
     <row r="107">
@@ -1814,10 +1814,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C107" s="2" t="n">
-        <v>0</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="108">
@@ -1827,10 +1827,10 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C108" s="2" t="n">
-        <v>0</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="109">
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C109" s="2" t="n">
         <v>0</v>
@@ -1853,7 +1853,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C110" s="2" t="n">
         <v>0</v>
@@ -1866,7 +1866,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C111" s="2" t="n">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C112" s="2" t="n">
         <v>0</v>
@@ -1888,222 +1888,222 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C113" s="2" t="n">
-        <v>0.022</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C114" s="2" t="n">
-        <v>0.118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C115" s="2" t="n">
-        <v>0.239</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C116" s="2" t="n">
-        <v>0.376</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C117" s="2" t="n">
-        <v>0.488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C118" s="2" t="n">
-        <v>0.548</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C119" s="2" t="n">
-        <v>0.5639999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C120" s="2" t="n">
-        <v>0.539</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C121" s="2" t="n">
-        <v>0.512</v>
+        <v>0.117</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C122" s="2" t="n">
-        <v>0.416</v>
+        <v>0.258</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C123" s="2" t="n">
-        <v>0.303</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C124" s="2" t="n">
-        <v>0.159</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C125" s="2" t="n">
-        <v>0.03</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C126" s="2" t="n">
-        <v>0</v>
+        <v>0.577</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C127" s="2" t="n">
-        <v>0</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C128" s="2" t="n">
-        <v>0</v>
+        <v>0.503</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C129" s="2" t="n">
-        <v>0</v>
+        <v>0.407</v>
       </c>
     </row>
     <row r="130">
@@ -2113,10 +2113,10 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C130" s="2" t="n">
-        <v>0</v>
+        <v>0.274</v>
       </c>
     </row>
     <row r="131">
@@ -2126,10 +2126,10 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C131" s="2" t="n">
-        <v>0</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="132">
@@ -2139,10 +2139,10 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C132" s="2" t="n">
-        <v>0</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="133">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C133" s="2" t="n">
         <v>0</v>
@@ -2165,7 +2165,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C134" s="2" t="n">
         <v>0</v>
@@ -2178,7 +2178,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C135" s="2" t="n">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C136" s="2" t="n">
         <v>0</v>
@@ -2200,222 +2200,222 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C137" s="2" t="n">
-        <v>0.024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C138" s="2" t="n">
-        <v>0.116</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C139" s="2" t="n">
-        <v>0.242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C140" s="2" t="n">
-        <v>0.383</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C141" s="2" t="n">
-        <v>0.506</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C142" s="2" t="n">
-        <v>0.552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C143" s="2" t="n">
-        <v>0.5639999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C144" s="2" t="n">
-        <v>0.539</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C145" s="2" t="n">
-        <v>0.486</v>
+        <v>0.117</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C146" s="2" t="n">
-        <v>0.385</v>
+        <v>0.244</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C147" s="2" t="n">
-        <v>0.274</v>
+        <v>0.383</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C148" s="2" t="n">
-        <v>0.162</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C149" s="2" t="n">
-        <v>0.028</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C150" s="2" t="n">
-        <v>0</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C151" s="2" t="n">
-        <v>0</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C152" s="2" t="n">
-        <v>0</v>
+        <v>0.489</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C153" s="2" t="n">
-        <v>0</v>
+        <v>0.388</v>
       </c>
     </row>
     <row r="154">
@@ -2425,10 +2425,10 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C154" s="2" t="n">
-        <v>0</v>
+        <v>0.279</v>
       </c>
     </row>
     <row r="155">
@@ -2438,10 +2438,10 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C155" s="2" t="n">
-        <v>0</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="156">
@@ -2451,10 +2451,10 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C156" s="2" t="n">
-        <v>0</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="157">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C157" s="2" t="n">
         <v>0</v>
@@ -2477,7 +2477,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C158" s="2" t="n">
         <v>0</v>
@@ -2490,7 +2490,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C159" s="2" t="n">
         <v>0</v>
@@ -2503,7 +2503,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C160" s="2" t="n">
         <v>0</v>
@@ -2512,131 +2512,131 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C161" s="2" t="n">
-        <v>0.028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C162" s="2" t="n">
-        <v>0.129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C163" s="2" t="n">
-        <v>0.268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C164" s="2" t="n">
-        <v>0.402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C165" s="2" t="n">
-        <v>0.506</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C166" s="2" t="n">
-        <v>0.5629999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C167" s="2" t="n">
-        <v>0.573</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C168" s="2" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C169" s="2" t="n">
-        <v>0.499</v>
+        <v>0.117</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C170" s="2" t="n">
-        <v>0.379</v>
+        <v>0.245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fetching the Volue and Transelectrica data
</commit_message>
<xml_diff>
--- a/Solina/Production/Results_Production_xgb.xlsx
+++ b/Solina/Production/Results_Production_xgb.xlsx
@@ -445,11 +445,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>0</v>
@@ -458,11 +458,11 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
@@ -471,128 +471,128 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.292</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.309</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.427</v>
+        <v>0.334</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.303</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.229</v>
+        <v>0.101</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.169</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.076</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0</v>
@@ -601,11 +601,11 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-05</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>0</v>
@@ -614,11 +614,11 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0</v>
@@ -627,11 +627,11 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2024-04-04</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
@@ -640,11 +640,11 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
@@ -653,11 +653,11 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
@@ -666,11 +666,11 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
@@ -679,11 +679,11 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>0</v>
@@ -692,11 +692,11 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
@@ -705,206 +705,206 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.014</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.055</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.112</v>
+        <v>0.316</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.19</v>
+        <v>0.365</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.262</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.312</v>
+        <v>0.349</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.385</v>
+        <v>0.261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0.403</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0.405</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>0.301</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0.189</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0.08699999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>0.015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>0</v>
@@ -913,11 +913,11 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-06</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
@@ -926,11 +926,11 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0</v>
@@ -939,11 +939,11 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>2024-04-05</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
@@ -952,11 +952,11 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>0</v>
@@ -965,11 +965,11 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>0</v>
@@ -978,11 +978,11 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>0</v>
@@ -991,11 +991,11 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>0</v>
@@ -1004,11 +1004,11 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>0</v>
@@ -1017,206 +1017,206 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>0</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>0</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>0.014</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>0.057</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0.15</v>
+        <v>0.491</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>0.219</v>
+        <v>0.536</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>0.284</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>0.365</v>
+        <v>0.578</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>0.397</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>0.38</v>
+        <v>0.415</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>0.321</v>
+        <v>0.297</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>0.217</v>
+        <v>0.167</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>0.146</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>0.012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>0</v>
@@ -1225,11 +1225,11 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-07</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>0</v>
@@ -1238,11 +1238,11 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>0</v>
@@ -1251,11 +1251,11 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>2024-04-06</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>0</v>
@@ -1264,11 +1264,11 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>0</v>
@@ -1277,11 +1277,11 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>0</v>
@@ -1290,11 +1290,11 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>0</v>
@@ -1303,11 +1303,11 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>0</v>
@@ -1316,11 +1316,11 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>0</v>
@@ -1329,206 +1329,206 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>0</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>0.019</v>
+        <v>0.269</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>0.11</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>0.241</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>0.359</v>
+        <v>0.594</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>0.515</v>
+        <v>0.589</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>0.57</v>
+        <v>0.582</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>0.573</v>
+        <v>0.534</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C79" s="2" t="n">
-        <v>0.572</v>
+        <v>0.428</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>0.498</v>
+        <v>0.305</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>0.388</v>
+        <v>0.179</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>0.26</v>
+        <v>0.037</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>0.139</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C84" s="2" t="n">
-        <v>0.023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>0</v>
@@ -1537,11 +1537,11 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C86" s="2" t="n">
         <v>0</v>
@@ -1550,11 +1550,11 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C87" s="2" t="n">
         <v>0</v>
@@ -1563,11 +1563,11 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>2024-04-07</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>0</v>
@@ -1576,11 +1576,11 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C89" s="2" t="n">
         <v>0</v>
@@ -1589,11 +1589,11 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>0</v>
@@ -1602,11 +1602,11 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C91" s="2" t="n">
         <v>0</v>
@@ -1615,11 +1615,11 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>0</v>
@@ -1628,11 +1628,11 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C93" s="2" t="n">
         <v>0</v>
@@ -1641,206 +1641,206 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C94" s="2" t="n">
-        <v>0</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C95" s="2" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C96" s="2" t="n">
-        <v>0.026</v>
+        <v>0.266</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C97" s="2" t="n">
-        <v>0.121</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C98" s="2" t="n">
-        <v>0.262</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C99" s="2" t="n">
-        <v>0.402</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C100" s="2" t="n">
-        <v>0.52</v>
+        <v>0.577</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C101" s="2" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C102" s="2" t="n">
-        <v>0.573</v>
+        <v>0.507</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C103" s="2" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.407</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C104" s="2" t="n">
-        <v>0.522</v>
+        <v>0.274</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C105" s="2" t="n">
-        <v>0.41</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C106" s="2" t="n">
-        <v>0.297</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C107" s="2" t="n">
-        <v>0.158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C108" s="2" t="n">
-        <v>0.027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C109" s="2" t="n">
         <v>0</v>
@@ -1849,11 +1849,11 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C110" s="2" t="n">
         <v>0</v>
@@ -1862,11 +1862,11 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C111" s="2" t="n">
         <v>0</v>
@@ -1875,11 +1875,11 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>2024-04-08</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C112" s="2" t="n">
         <v>0</v>
@@ -1888,11 +1888,11 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C113" s="2" t="n">
         <v>0</v>
@@ -1901,11 +1901,11 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C114" s="2" t="n">
         <v>0</v>
@@ -1914,11 +1914,11 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C115" s="2" t="n">
         <v>0</v>
@@ -1927,11 +1927,11 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C116" s="2" t="n">
         <v>0</v>
@@ -1940,11 +1940,11 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C117" s="2" t="n">
         <v>0</v>
@@ -1953,206 +1953,206 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C118" s="2" t="n">
-        <v>0</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C119" s="2" t="n">
-        <v>0</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C120" s="2" t="n">
-        <v>0.027</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C121" s="2" t="n">
-        <v>0.117</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C122" s="2" t="n">
-        <v>0.258</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C123" s="2" t="n">
-        <v>0.402</v>
+        <v>0.5580000000000001</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C124" s="2" t="n">
-        <v>0.52</v>
+        <v>0.581</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C125" s="2" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.575</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C126" s="2" t="n">
-        <v>0.577</v>
+        <v>0.503</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C127" s="2" t="n">
-        <v>0.573</v>
+        <v>0.388</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C128" s="2" t="n">
-        <v>0.503</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C129" s="2" t="n">
-        <v>0.407</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C130" s="2" t="n">
-        <v>0.274</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C131" s="2" t="n">
-        <v>0.151</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C132" s="2" t="n">
-        <v>0.028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C133" s="2" t="n">
         <v>0</v>
@@ -2161,11 +2161,11 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-10</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C134" s="2" t="n">
         <v>0</v>
@@ -2174,11 +2174,11 @@
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C135" s="2" t="n">
         <v>0</v>
@@ -2187,11 +2187,11 @@
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>2024-04-09</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C136" s="2" t="n">
         <v>0</v>
@@ -2200,11 +2200,11 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C137" s="2" t="n">
         <v>0</v>
@@ -2213,11 +2213,11 @@
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C138" s="2" t="n">
         <v>0</v>
@@ -2226,11 +2226,11 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C139" s="2" t="n">
         <v>0</v>
@@ -2239,11 +2239,11 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C140" s="2" t="n">
         <v>0</v>
@@ -2252,11 +2252,11 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C141" s="2" t="n">
         <v>0</v>
@@ -2265,206 +2265,206 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C142" s="2" t="n">
-        <v>0</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C143" s="2" t="n">
-        <v>0</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C144" s="2" t="n">
-        <v>0.027</v>
+        <v>0.225</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C145" s="2" t="n">
-        <v>0.117</v>
+        <v>0.363</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C146" s="2" t="n">
-        <v>0.244</v>
+        <v>0.477</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C147" s="2" t="n">
-        <v>0.383</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C148" s="2" t="n">
-        <v>0.506</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C149" s="2" t="n">
-        <v>0.548</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C150" s="2" t="n">
-        <v>0.573</v>
+        <v>0.459</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C151" s="2" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C152" s="2" t="n">
-        <v>0.489</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C153" s="2" t="n">
-        <v>0.388</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C154" s="2" t="n">
-        <v>0.279</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C155" s="2" t="n">
-        <v>0.156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C156" s="2" t="n">
-        <v>0.029</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C157" s="2" t="n">
         <v>0</v>
@@ -2473,11 +2473,11 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-11</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C158" s="2" t="n">
         <v>0</v>
@@ -2486,11 +2486,11 @@
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C159" s="2" t="n">
         <v>0</v>
@@ -2499,11 +2499,11 @@
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C160" s="2" t="n">
         <v>0</v>
@@ -2512,11 +2512,11 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C161" s="2" t="n">
         <v>0</v>
@@ -2525,11 +2525,11 @@
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C162" s="2" t="n">
         <v>0</v>
@@ -2538,11 +2538,11 @@
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C163" s="2" t="n">
         <v>0</v>
@@ -2551,11 +2551,11 @@
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C164" s="2" t="n">
         <v>0</v>
@@ -2564,11 +2564,11 @@
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C165" s="2" t="n">
         <v>0</v>
@@ -2577,66 +2577,66 @@
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C166" s="2" t="n">
-        <v>0</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C167" s="2" t="n">
-        <v>0</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C168" s="2" t="n">
-        <v>0.028</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C169" s="2" t="n">
-        <v>0.117</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>2024-04-11</t>
+          <t>2024-04-12</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C170" s="2" t="n">
-        <v>0.245</v>
+        <v>0.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>